<commit_message>
Update BASE DE DADOS.ACHAR-PASTAS.Copia.xlsx
</commit_message>
<xml_diff>
--- a/BASE DE DADOS.ACHAR-PASTAS.Copia.xlsx
+++ b/BASE DE DADOS.ACHAR-PASTAS.Copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.dossantos\Favorites\PYTHON\TESTES AUTOMAÇÃO PYAUTOGUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.dossantos\Favorites\PYTHON\GITHUB\CODES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF09B72-C88F-45A5-A15E-333AD25240F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5696E75-4825-4FF9-8950-D9095494DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,11 +417,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>130339</v>
+        <v>120339</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="2"/>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>120340</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>

</xml_diff>